<commit_message>
working on building scene
</commit_message>
<xml_diff>
--- a/cost.xlsx
+++ b/cost.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pascaljardin/Documents/GitHub/Lady-Justice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CE46D5-982A-3145-B727-34FED3C65AFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5781C4C5-3ECC-124C-A7D0-4013EF554B4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" xr2:uid="{55078296-9595-B04F-89F8-C73D7D3F7192}"/>
   </bookViews>
@@ -538,7 +538,7 @@
       <c r="F4" s="6"/>
       <c r="L4">
         <f>SUM(B3:B24)</f>
-        <v>27.5</v>
+        <v>29</v>
       </c>
       <c r="M4" t="s">
         <v>8</v>
@@ -551,7 +551,7 @@
       </c>
       <c r="P4" s="5">
         <f>L4*N4</f>
-        <v>550</v>
+        <v>580</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -616,14 +616,14 @@
       </c>
       <c r="M9" s="4">
         <f>SUM(H5:H7) + P4</f>
-        <v>626.5</v>
+        <v>656.5</v>
       </c>
       <c r="O9" t="s">
         <v>15</v>
       </c>
       <c r="P9" s="4">
         <f>M9-SUM(M13:M21)</f>
-        <v>426.5</v>
+        <v>456.5</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -643,6 +643,12 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>43925</v>
+      </c>
+      <c r="B12">
+        <v>1.5</v>
+      </c>
       <c r="L12" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Worked on in and out
Worked on in and out
</commit_message>
<xml_diff>
--- a/cost.xlsx
+++ b/cost.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pascaljardin/Documents/GitHub/Lady-Justice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B00473-FB65-3A49-82F7-28A25C9B0301}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BEC97F-0FB4-9B45-ADB9-449B085EEB7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6760" yWindow="6560" windowWidth="28040" windowHeight="17440" xr2:uid="{55078296-9595-B04F-89F8-C73D7D3F7192}"/>
   </bookViews>
@@ -484,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB61B247-2104-BC45-AE50-878C86EE91AF}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,7 +538,7 @@
       <c r="F4" s="6"/>
       <c r="L4">
         <f>SUM(B3:B24)</f>
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="M4" t="s">
         <v>8</v>
@@ -551,7 +551,7 @@
       </c>
       <c r="P4" s="5">
         <f>L4*N4</f>
-        <v>1080</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -616,14 +616,14 @@
       </c>
       <c r="M9" s="4">
         <f>SUM(H5:H7) + P4</f>
-        <v>1156.5</v>
+        <v>1276.5</v>
       </c>
       <c r="O9" t="s">
         <v>15</v>
       </c>
       <c r="P9" s="4">
         <f>M9-SUM(M13:M21)</f>
-        <v>456.5</v>
+        <v>576.5</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -733,6 +733,30 @@
       </c>
       <c r="B20">
         <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>43936</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>43938</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>